<commit_message>
remove name column from activity_check table Check in Activity is done
</commit_message>
<xml_diff>
--- a/public/example/namelist_example.xlsx
+++ b/public/example/namelist_example.xlsx
@@ -33,15 +33,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>職位</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>電話</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>信箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>職位、票種</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -448,7 +448,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -468,13 +468,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">

</xml_diff>